<commit_message>
added images for visualization
</commit_message>
<xml_diff>
--- a/Abstract-Feature-Extraction/ModelLog.xlsx
+++ b/Abstract-Feature-Extraction/ModelLog.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selenaling/Documents/Unnnnndergraduate/2018_EvolutionaryArt/Generative-Art-Research/Abstract-Feature-Extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zling/Desktop/Generative-Art-Research/Abstract-Feature-Extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>711Train_vgg10ep</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Use mse loss function instead of custom function</t>
   </si>
   <si>
-    <t>718Trin_ctm100ep_rd</t>
-  </si>
-  <si>
     <t>Use Hans' Model with built-in loss function</t>
   </si>
   <si>
@@ -151,6 +148,18 @@
   </si>
   <si>
     <t>plot showing fit distribution; evo-art prediction show some outliers;</t>
+  </si>
+  <si>
+    <t>718Train_ctm100ep_rd</t>
+  </si>
+  <si>
+    <t>815Train_ctm200ep_rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As above </t>
+  </si>
+  <si>
+    <t>Added 867 blank images as r=0</t>
   </si>
 </sst>
 </file>
@@ -477,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,21 +646,32 @@
         <v>32</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add scrollable feature to the visualization applet
</commit_message>
<xml_diff>
--- a/Abstract-Feature-Extraction/ModelLog.xlsx
+++ b/Abstract-Feature-Extraction/ModelLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="24740" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="-49900" yWindow="460" windowWidth="46240" windowHeight="25960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>711Train_vgg10ep</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Added another FC layer (512)</t>
   </si>
   <si>
-    <t>✔；looks good</t>
-  </si>
-  <si>
     <t>712Train_vgg10ep</t>
   </si>
   <si>
@@ -80,89 +77,106 @@
     <t xml:space="preserve">Regenerated Rd_Smooth image sets with png format; </t>
   </si>
   <si>
-    <t>✔; have some abnormity: Rd_Smooth image sets give large error</t>
-  </si>
-  <si>
     <t xml:space="preserve">Same as above; Just training for more epochs; </t>
   </si>
   <si>
-    <t>✔; Rd_Smooth image still give poor results than others</t>
-  </si>
-  <si>
     <t>712Train_vgg100ep (GPU 0)</t>
   </si>
   <si>
-    <t>✔；trained on the wrong image set ✖️</t>
-  </si>
-  <si>
     <t>713Train_vgg26ep_col</t>
   </si>
   <si>
-    <t xml:space="preserve">✔；
+    <t>Revised the loss function so that it considers 
+the batch size to be 100 instead of 300</t>
+  </si>
+  <si>
+    <t>No change;</t>
+  </si>
+  <si>
+    <t>713Train_vgg100ep</t>
+  </si>
+  <si>
+    <t>713Train_nvgg100ep_col</t>
+  </si>
+  <si>
+    <t>717Train_vgg100ep_rd</t>
+  </si>
+  <si>
+    <t>Only Roundness Images (no smooth image, only blurred strokes)</t>
+  </si>
+  <si>
+    <t>Use mse loss function instead of custom function</t>
+  </si>
+  <si>
+    <t>Use Hans' Model with built-in loss function</t>
+  </si>
+  <si>
+    <t>recognize the smooth shape better; plot not showing super fit distribtuion</t>
+  </si>
+  <si>
+    <t>plot showing fit distribution; evo-art prediction show some outliers;</t>
+  </si>
+  <si>
+    <t>718Train_ctm100ep_rd</t>
+  </si>
+  <si>
+    <t>815Train_ctm200ep_rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As above </t>
+  </si>
+  <si>
+    <t>Added 867 blank images as r=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analyzed heatmaps shows lower value for blank regions; </t>
+  </si>
+  <si>
+    <t>817Train_ctm200ep_rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactored processing code so that the stroke color and background color differ by at least 70; 
+removed images with blur=3/4; </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> recognizes the inner noise better! 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R: recognizes overall roundness better; 
+still bad at recognize the color-smooth round shapes;
+M: personally wouldn’t agree with the prediction 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Weird patterns, reach a flat plateau in messiness prediction; 
 might be the problem of loss function???
 Prediction Visualization shows better recognition of complexity within a central area; </t>
   </si>
   <si>
-    <t>✔；</t>
-  </si>
-  <si>
-    <t>Revised the loss function so that it considers 
-the batch size to be 100 instead of 300</t>
-  </si>
-  <si>
-    <t>No change;</t>
-  </si>
-  <si>
-    <t>713Train_vgg100ep</t>
-  </si>
-  <si>
-    <t>713Train_nvgg100ep_col</t>
-  </si>
-  <si>
-    <t xml:space="preserve">✔； 
-R: recognizes overall roundness better; 
-still bad at recognize the color-smooth round shapes;
-M: personally wouldn’t agree with the prediction 
+    <t>Rd_Smooth image still give poor results than others</t>
+  </si>
+  <si>
+    <t>trained on the wrong image set ✖️</t>
+  </si>
+  <si>
+    <t>looks good</t>
+  </si>
+  <si>
+    <t>have some abnormity: Rd_Smooth image sets give large error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower test score -&gt; less data images?;
+Recognizes the inperceptiable gradients less, especially with "Images/evo_art_test/Image-1.jpg";
+Gives much lower score to blurred circles, shown by "evo_art_test/image-49.jpg"
 </t>
   </si>
   <si>
-    <t xml:space="preserve">✔； 
-recognizes the inner noise better! 
-</t>
-  </si>
-  <si>
-    <t>717Train_vgg100ep_rd</t>
-  </si>
-  <si>
-    <t>Only Roundness Images (no smooth image, only blurred strokes)</t>
-  </si>
-  <si>
-    <t>Use mse loss function instead of custom function</t>
-  </si>
-  <si>
-    <t>Use Hans' Model with built-in loss function</t>
-  </si>
-  <si>
-    <t>recognize the smooth shape better; plot not showing super fit distribtuion</t>
-  </si>
-  <si>
-    <t>plot showing fit distribution; evo-art prediction show some outliers;</t>
-  </si>
-  <si>
-    <t>718Train_ctm100ep_rd</t>
-  </si>
-  <si>
-    <t>815Train_ctm200ep_rd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As above </t>
-  </si>
-  <si>
-    <t>Added 867 blank images as r=0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">analyzed heatmaps shows lower value for blank regions; </t>
+    <t>818Train_ctm200ep_rd</t>
+  </si>
+  <si>
+    <t>added images with blur=3/4 but with heavier stroke weights;</t>
   </si>
 </sst>
 </file>
@@ -489,17 +503,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" style="2" customWidth="1"/>
     <col min="2" max="2" width="47.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="65.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="83.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="55.33203125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
@@ -537,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -551,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -565,119 +579,141 @@
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="115" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="10" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>